<commit_message>
Updates to data, and enhanced PW Calc Algorithm
</commit_message>
<xml_diff>
--- a/Person_B_and_trucks/on_trucks/Processed_Standalone/12_455-55R22.xlsx
+++ b/Person_B_and_trucks/on_trucks/Processed_Standalone/12_455-55R22.xlsx
@@ -408,40 +408,43 @@
     <t>signal segment 10</t>
   </si>
   <si>
+    <t>First_Noticeable_Increase_Cumulative_Value</t>
+  </si>
+  <si>
+    <t>First_Noticeable_Increase_Index</t>
+  </si>
+  <si>
     <t>Intensity_Threshold</t>
   </si>
   <si>
-    <t>First_Noticeable_Increase_Index</t>
+    <t>Point_Exceeds_Cumulative_Value</t>
   </si>
   <si>
     <t>Point_Exceeds_Index</t>
   </si>
   <si>
-    <t>First_Noticeable_Increase_Cumulative_Value</t>
-  </si>
-  <si>
-    <t>Point_Exceeds_Cumulative_Value</t>
+    <t>Pressure</t>
   </si>
   <si>
     <t>Pulse_Width</t>
   </si>
   <si>
+    <t>Rim</t>
+  </si>
+  <si>
+    <t>TireSize</t>
+  </si>
+  <si>
     <t>Tire_Number</t>
   </si>
   <si>
-    <t>Pressure</t>
-  </si>
-  <si>
-    <t>TireSize</t>
-  </si>
-  <si>
     <t>Tire_Type</t>
   </si>
   <si>
     <t>Wear</t>
   </si>
   <si>
-    <t>Rim</t>
+    <t>Ir</t>
   </si>
   <si>
     <t>455-55R22.5</t>
@@ -451,9 +454,6 @@
   </si>
   <si>
     <t>0%</t>
-  </si>
-  <si>
-    <t>Ir</t>
   </si>
 </sst>
 </file>
@@ -1433,100 +1433,100 @@
         <v>0</v>
       </c>
       <c r="CH2">
-        <v>0.2249777582959693</v>
+        <v>0.3047491211860124</v>
       </c>
       <c r="CI2">
-        <v>0.2695762577496729</v>
+        <v>0.3744563207841319</v>
       </c>
       <c r="CJ2">
-        <v>0.1022378216958758</v>
+        <v>0.1129073022000434</v>
       </c>
       <c r="CK2">
-        <v>0.009304663203275268</v>
+        <v>0</v>
       </c>
       <c r="CL2">
-        <v>0.03745639972338249</v>
+        <v>0.01165431012630232</v>
       </c>
       <c r="CM2">
-        <v>0.002857822867674904</v>
+        <v>0</v>
       </c>
       <c r="CN2">
-        <v>0.004925485919507793</v>
+        <v>0</v>
       </c>
       <c r="CO2">
-        <v>0.005082872498054075</v>
+        <v>0</v>
       </c>
       <c r="CP2">
-        <v>0.01176367037736587</v>
+        <v>0</v>
       </c>
       <c r="CQ2">
-        <v>1.363519110457816E-05</v>
+        <v>0</v>
       </c>
       <c r="CR2">
-        <v>0.01139366810246692</v>
+        <v>0</v>
       </c>
       <c r="CS2">
-        <v>0.1347736568279998</v>
+        <v>0.1637606264469902</v>
       </c>
       <c r="CT2">
-        <v>0.0001756367451645541</v>
+        <v>0</v>
       </c>
       <c r="CU2">
-        <v>0.0507757121355001</v>
+        <v>0.0324723192565196</v>
       </c>
       <c r="CV2">
-        <v>0.007099346328404574</v>
+        <v>0</v>
       </c>
       <c r="CW2">
-        <v>0.01379541050045922</v>
+        <v>0</v>
       </c>
       <c r="CX2">
-        <v>0.02444058621326464</v>
+        <v>0</v>
       </c>
       <c r="CY2">
-        <v>8.417643049573597E-06</v>
+        <v>0</v>
       </c>
       <c r="CZ2">
-        <v>0.005781907734067388</v>
+        <v>0</v>
       </c>
       <c r="DA2">
-        <v>0.01399531909463761</v>
+        <v>0</v>
       </c>
       <c r="DB2">
-        <v>6.461167766009255E-05</v>
+        <v>0</v>
       </c>
       <c r="DC2">
-        <v>0.02686143504238039</v>
+        <v>0</v>
       </c>
       <c r="DD2">
-        <v>0.002673279196723928</v>
+        <v>0</v>
       </c>
       <c r="DE2">
-        <v>0.005579702131621142</v>
+        <v>0</v>
       </c>
       <c r="DF2">
-        <v>0.001656926074692258</v>
+        <v>0</v>
       </c>
       <c r="DG2">
-        <v>0.0132674342338117</v>
+        <v>0</v>
       </c>
       <c r="DH2">
-        <v>0.00878364350700651</v>
+        <v>0</v>
       </c>
       <c r="DI2">
-        <v>0.0005844612168661797</v>
+        <v>0</v>
       </c>
       <c r="DJ2">
-        <v>0.0001806803315175779</v>
+        <v>0</v>
       </c>
       <c r="DK2">
-        <v>0.003890820092055884</v>
+        <v>0</v>
       </c>
       <c r="DL2">
-        <v>0.005816092352536995</v>
+        <v>0</v>
       </c>
       <c r="DM2">
-        <v>0.0002048652962300886</v>
+        <v>0</v>
       </c>
       <c r="DN2">
         <v>0</v>
@@ -1792,100 +1792,100 @@
         <v>0</v>
       </c>
       <c r="CH3">
-        <v>0.1479818478787089</v>
+        <v>0.208813990958931</v>
       </c>
       <c r="CI3">
-        <v>0.2650756834505651</v>
+        <v>0.4168016476780347</v>
       </c>
       <c r="CJ3">
-        <v>0.07659005594236251</v>
+        <v>0.08200448436704529</v>
       </c>
       <c r="CK3">
-        <v>0.01365988213917466</v>
+        <v>0</v>
       </c>
       <c r="CL3">
-        <v>0.02321236656201623</v>
+        <v>0</v>
       </c>
       <c r="CM3">
-        <v>0.003356964808872546</v>
+        <v>0</v>
       </c>
       <c r="CN3">
-        <v>0.02465153904851867</v>
+        <v>0</v>
       </c>
       <c r="CO3">
-        <v>0.01054578309910426</v>
+        <v>0</v>
       </c>
       <c r="CP3">
-        <v>0.02397857417489206</v>
+        <v>0</v>
       </c>
       <c r="CQ3">
-        <v>0.001099741592538775</v>
+        <v>0</v>
       </c>
       <c r="CR3">
-        <v>0.02463680852153297</v>
+        <v>0</v>
       </c>
       <c r="CS3">
-        <v>0.1428302041733386</v>
+        <v>0.1996633956496317</v>
       </c>
       <c r="CT3">
-        <v>0.007088627402992534</v>
+        <v>0</v>
       </c>
       <c r="CU3">
-        <v>0.06551930807566718</v>
+        <v>0.06234009387478088</v>
       </c>
       <c r="CV3">
-        <v>0.01991949301466354</v>
+        <v>0</v>
       </c>
       <c r="CW3">
-        <v>0.006361796904641412</v>
+        <v>0</v>
       </c>
       <c r="CX3">
-        <v>0.04752423547913006</v>
+        <v>0.0303763874715764</v>
       </c>
       <c r="CY3">
-        <v>0.0002740933742739271</v>
+        <v>0</v>
       </c>
       <c r="CZ3">
-        <v>0.00592553128907894</v>
+        <v>0</v>
       </c>
       <c r="DA3">
-        <v>0.01784670262385884</v>
+        <v>0</v>
       </c>
       <c r="DB3">
-        <v>5.663086747130661E-05</v>
+        <v>0</v>
       </c>
       <c r="DC3">
-        <v>0.02624787492678387</v>
+        <v>0</v>
       </c>
       <c r="DD3">
-        <v>0.004872046972007204</v>
+        <v>0</v>
       </c>
       <c r="DE3">
-        <v>0.0007089465482321764</v>
+        <v>0</v>
       </c>
       <c r="DF3">
-        <v>0.002059592779326806</v>
+        <v>0</v>
       </c>
       <c r="DG3">
-        <v>0.01613111575369115</v>
+        <v>0</v>
       </c>
       <c r="DH3">
-        <v>0.0109085523644295</v>
+        <v>0</v>
       </c>
       <c r="DI3">
-        <v>7.743596447185659E-05</v>
+        <v>0</v>
       </c>
       <c r="DJ3">
-        <v>0.001496920984070251</v>
+        <v>0</v>
       </c>
       <c r="DK3">
-        <v>0.004383941232629689</v>
+        <v>0</v>
       </c>
       <c r="DL3">
-        <v>0.002790585239489691</v>
+        <v>0</v>
       </c>
       <c r="DM3">
-        <v>0.002187116811464971</v>
+        <v>0</v>
       </c>
       <c r="DN3">
         <v>0</v>
@@ -2154,100 +2154,100 @@
         <v>0</v>
       </c>
       <c r="CI4">
-        <v>0.1196721865236701</v>
+        <v>0.1671051085991076</v>
       </c>
       <c r="CJ4">
-        <v>0.00379078349905809</v>
+        <v>0</v>
       </c>
       <c r="CK4">
-        <v>0.2511109330030337</v>
+        <v>0.4120426623272856</v>
       </c>
       <c r="CL4">
-        <v>0.01064821629726815</v>
+        <v>0</v>
       </c>
       <c r="CM4">
-        <v>0.0102572105627424</v>
+        <v>0</v>
       </c>
       <c r="CN4">
-        <v>0.02823462477596669</v>
+        <v>0</v>
       </c>
       <c r="CO4">
-        <v>0.007017976766069078</v>
+        <v>0</v>
       </c>
       <c r="CP4">
-        <v>0.01646680932530454</v>
+        <v>0</v>
       </c>
       <c r="CQ4">
-        <v>5.60438542915847E-05</v>
+        <v>0</v>
       </c>
       <c r="CR4">
-        <v>0.04265585655940853</v>
+        <v>0.02358432828239834</v>
       </c>
       <c r="CS4">
-        <v>6.147148946993795E-05</v>
+        <v>0</v>
       </c>
       <c r="CT4">
-        <v>0.1035683338162758</v>
+        <v>0.1370954014663076</v>
       </c>
       <c r="CU4">
-        <v>0.1173680066612781</v>
+        <v>0.1628112440122856</v>
       </c>
       <c r="CV4">
-        <v>0.03782449940282823</v>
+        <v>0.01458104093511905</v>
       </c>
       <c r="CW4">
-        <v>0.02269888158461807</v>
+        <v>0</v>
       </c>
       <c r="CX4">
-        <v>0.06366644628657096</v>
+        <v>0.06273779396890761</v>
       </c>
       <c r="CY4">
-        <v>0.0001843430994722521</v>
+        <v>0</v>
       </c>
       <c r="CZ4">
-        <v>0.03484155189646336</v>
+        <v>0.009022285357491172</v>
       </c>
       <c r="DA4">
-        <v>0.006614545370932591</v>
+        <v>0</v>
       </c>
       <c r="DB4">
-        <v>0.0001762598416099902</v>
+        <v>0</v>
       </c>
       <c r="DC4">
-        <v>0.03062779975846153</v>
+        <v>0.001169911774020542</v>
       </c>
       <c r="DD4">
-        <v>0.002103471684714524</v>
+        <v>0</v>
       </c>
       <c r="DE4">
-        <v>0.008325746933253447</v>
+        <v>0</v>
       </c>
       <c r="DF4">
-        <v>0.0005050471127641088</v>
+        <v>0</v>
       </c>
       <c r="DG4">
-        <v>0.004053761354086464</v>
+        <v>0</v>
       </c>
       <c r="DH4">
-        <v>0.021628719198779</v>
+        <v>0</v>
       </c>
       <c r="DI4">
-        <v>0.03528584114756692</v>
+        <v>0.009850223277076523</v>
       </c>
       <c r="DJ4">
-        <v>0.006121756527050846</v>
+        <v>0</v>
       </c>
       <c r="DK4">
-        <v>0.001155521678249587</v>
+        <v>0</v>
       </c>
       <c r="DL4">
-        <v>0.006801882048346268</v>
+        <v>0</v>
       </c>
       <c r="DM4">
-        <v>0.005953905332209793</v>
+        <v>0</v>
       </c>
       <c r="DN4">
-        <v>0.0005215666081855738</v>
+        <v>0</v>
       </c>
       <c r="DO4">
         <v>0</v>
@@ -2513,100 +2513,100 @@
         <v>0</v>
       </c>
       <c r="CI5">
-        <v>0.1681583925085048</v>
+        <v>0.2609878969724378</v>
       </c>
       <c r="CJ5">
-        <v>0.003381716421389815</v>
+        <v>0</v>
       </c>
       <c r="CK5">
-        <v>0.2494511188919347</v>
+        <v>0.4145537955960857</v>
       </c>
       <c r="CL5">
-        <v>0.0180035641464265</v>
+        <v>0</v>
       </c>
       <c r="CM5">
-        <v>0.03930849679519008</v>
+        <v>0.0175842014259234</v>
       </c>
       <c r="CN5">
-        <v>0.03296281282604691</v>
+        <v>0.005596896971317508</v>
       </c>
       <c r="CO5">
-        <v>3.60071615006932E-06</v>
+        <v>0</v>
       </c>
       <c r="CP5">
-        <v>0.01080460981532327</v>
+        <v>0</v>
       </c>
       <c r="CQ5">
-        <v>0.01404442094428954</v>
+        <v>0</v>
       </c>
       <c r="CR5">
-        <v>0.01799369256246432</v>
+        <v>0</v>
       </c>
       <c r="CS5">
-        <v>0.0005035198101016438</v>
+        <v>0</v>
       </c>
       <c r="CT5">
-        <v>0.07571930623503023</v>
+        <v>0.08636598449554833</v>
       </c>
       <c r="CU5">
-        <v>0.07299800564366386</v>
+        <v>0.08122531583637267</v>
       </c>
       <c r="CV5">
-        <v>0.04442872954843887</v>
+        <v>0.02725656916281305</v>
       </c>
       <c r="CW5">
-        <v>0.01445507396663298</v>
+        <v>0</v>
       </c>
       <c r="CX5">
-        <v>0.08634018526181785</v>
+        <v>0.1064293395395015</v>
       </c>
       <c r="CY5">
-        <v>0.001828145465890909</v>
+        <v>0</v>
       </c>
       <c r="CZ5">
-        <v>0.01713676646006991</v>
+        <v>0</v>
       </c>
       <c r="DA5">
-        <v>0.02356360817679539</v>
+        <v>0</v>
       </c>
       <c r="DB5">
-        <v>0.000461510984573099</v>
+        <v>0</v>
       </c>
       <c r="DC5">
-        <v>0.01932017531137013</v>
+        <v>0</v>
       </c>
       <c r="DD5">
-        <v>0.01437671630413597</v>
+        <v>0</v>
       </c>
       <c r="DE5">
-        <v>0.01907401666127936</v>
+        <v>0</v>
       </c>
       <c r="DF5">
-        <v>0.003845954278829865</v>
+        <v>0</v>
       </c>
       <c r="DG5">
-        <v>0.000614518167160948</v>
+        <v>0</v>
       </c>
       <c r="DH5">
-        <v>0.006395008016957067</v>
+        <v>0</v>
       </c>
       <c r="DI5">
-        <v>0.02864911881233556</v>
+        <v>0</v>
       </c>
       <c r="DJ5">
-        <v>0.00448785231023218</v>
+        <v>0</v>
       </c>
       <c r="DK5">
-        <v>3.356801685818977E-06</v>
+        <v>0</v>
       </c>
       <c r="DL5">
-        <v>0.003455401519385688</v>
+        <v>0</v>
       </c>
       <c r="DM5">
-        <v>0.007563501145347743</v>
+        <v>0</v>
       </c>
       <c r="DN5">
-        <v>0.0006671034905447868</v>
+        <v>0</v>
       </c>
       <c r="DO5">
         <v>0</v>
@@ -2869,100 +2869,100 @@
         <v>0</v>
       </c>
       <c r="CH6">
-        <v>0.2303706899218832</v>
+        <v>0.3505469830983896</v>
       </c>
       <c r="CI6">
-        <v>0.04056451312503274</v>
+        <v>0.01848253457293261</v>
       </c>
       <c r="CJ6">
-        <v>0.1084231465479497</v>
+        <v>0.1372006925672828</v>
       </c>
       <c r="CK6">
-        <v>0.0001206910458220724</v>
+        <v>0</v>
       </c>
       <c r="CL6">
-        <v>0.037392306915014</v>
+        <v>0.01293278417220497</v>
       </c>
       <c r="CM6">
-        <v>0.03350774338625926</v>
+        <v>0.006136770113512589</v>
       </c>
       <c r="CN6">
-        <v>0.02519014397164324</v>
+        <v>0</v>
       </c>
       <c r="CO6">
-        <v>0.003446687825673967</v>
+        <v>0</v>
       </c>
       <c r="CP6">
-        <v>0.001534663045495246</v>
+        <v>0</v>
       </c>
       <c r="CQ6">
-        <v>0.0188816194732402</v>
+        <v>0</v>
       </c>
       <c r="CR6">
-        <v>0.0004910756271179226</v>
+        <v>0</v>
       </c>
       <c r="CS6">
-        <v>0.1211042825232054</v>
+        <v>0.1593862425602454</v>
       </c>
       <c r="CT6">
-        <v>0.03723427238010964</v>
+        <v>0.01265630396715263</v>
       </c>
       <c r="CU6">
-        <v>0.1122762319727184</v>
+        <v>0.1439416359248149</v>
       </c>
       <c r="CV6">
-        <v>2.18826300283937E-07</v>
+        <v>0</v>
       </c>
       <c r="CW6">
-        <v>0.1207212059419259</v>
+        <v>0.1587160530234647</v>
       </c>
       <c r="CX6">
-        <v>0.0286779306238306</v>
+        <v>0</v>
       </c>
       <c r="CY6">
-        <v>0.01521582726947954</v>
+        <v>0</v>
       </c>
       <c r="CZ6">
-        <v>0.01054248206366118</v>
+        <v>0</v>
       </c>
       <c r="DA6">
-        <v>0.00587468231352364</v>
+        <v>0</v>
       </c>
       <c r="DB6">
-        <v>0.006749384387147781</v>
+        <v>0</v>
       </c>
       <c r="DC6">
-        <v>0.008792124250053287</v>
+        <v>0</v>
       </c>
       <c r="DD6">
-        <v>0.000503357666639423</v>
+        <v>0</v>
       </c>
       <c r="DE6">
-        <v>0.001972028703693788</v>
+        <v>0</v>
       </c>
       <c r="DF6">
-        <v>0.005270231014160762</v>
+        <v>0</v>
       </c>
       <c r="DG6">
-        <v>0.002477041657308433</v>
+        <v>0</v>
       </c>
       <c r="DH6">
-        <v>0.0129233163084829</v>
+        <v>0</v>
       </c>
       <c r="DI6">
-        <v>0.001339479555217731</v>
+        <v>0</v>
       </c>
       <c r="DJ6">
-        <v>0.001280843639323974</v>
+        <v>0</v>
       </c>
       <c r="DK6">
-        <v>0.004550960643992668</v>
+        <v>0</v>
       </c>
       <c r="DL6">
-        <v>0.0001022347785816617</v>
+        <v>0</v>
       </c>
       <c r="DM6">
-        <v>0.002468582595511672</v>
+        <v>0</v>
       </c>
       <c r="DN6">
         <v>0</v>
@@ -3228,100 +3228,100 @@
         <v>0</v>
       </c>
       <c r="CH7">
-        <v>0.2532391155057309</v>
+        <v>0.3918612947215527</v>
       </c>
       <c r="CI7">
-        <v>0.04447334778652063</v>
+        <v>0.02540569465047757</v>
       </c>
       <c r="CJ7">
-        <v>0.1905812226695157</v>
+        <v>0.2818751798075055</v>
       </c>
       <c r="CK7">
-        <v>0.01041160995326073</v>
+        <v>0</v>
       </c>
       <c r="CL7">
-        <v>0.0102449082371535</v>
+        <v>0</v>
       </c>
       <c r="CM7">
-        <v>0.06234902140424754</v>
+        <v>0.05678363929066113</v>
       </c>
       <c r="CN7">
-        <v>0.002776040593503857</v>
+        <v>0</v>
       </c>
       <c r="CO7">
-        <v>0.007446147438323871</v>
+        <v>0</v>
       </c>
       <c r="CP7">
-        <v>0.0002360193314504686</v>
+        <v>0</v>
       </c>
       <c r="CQ7">
-        <v>0.0241304055070446</v>
+        <v>0</v>
       </c>
       <c r="CR7">
-        <v>0.01403719128473547</v>
+        <v>0</v>
       </c>
       <c r="CS7">
-        <v>0.1104810316203824</v>
+        <v>0.1412718428840023</v>
       </c>
       <c r="CT7">
-        <v>0.013734491341096</v>
+        <v>0</v>
       </c>
       <c r="CU7">
-        <v>0.04835991025596051</v>
+        <v>0.03222794619828845</v>
       </c>
       <c r="CV7">
-        <v>0.00416964577285128</v>
+        <v>0</v>
       </c>
       <c r="CW7">
-        <v>0.0702054691084591</v>
+        <v>0.07057440244751247</v>
       </c>
       <c r="CX7">
-        <v>0.0162821826587384</v>
+        <v>0</v>
       </c>
       <c r="CY7">
-        <v>0.02464533148433878</v>
+        <v>0</v>
       </c>
       <c r="CZ7">
-        <v>0.003197731653662381</v>
+        <v>0</v>
       </c>
       <c r="DA7">
-        <v>0.00101894769655745</v>
+        <v>0</v>
       </c>
       <c r="DB7">
-        <v>0.02142946727820063</v>
+        <v>0</v>
       </c>
       <c r="DC7">
-        <v>0.006775600652958178</v>
+        <v>0</v>
       </c>
       <c r="DD7">
-        <v>0.01515499375460635</v>
+        <v>0</v>
       </c>
       <c r="DE7">
-        <v>0.002500264862940761</v>
+        <v>0</v>
       </c>
       <c r="DF7">
-        <v>0.003352775509006984</v>
+        <v>0</v>
       </c>
       <c r="DG7">
-        <v>0.00290802737837411</v>
+        <v>0</v>
       </c>
       <c r="DH7">
-        <v>0.02234980464525121</v>
+        <v>0</v>
       </c>
       <c r="DI7">
-        <v>0.002933116282797513</v>
+        <v>0</v>
       </c>
       <c r="DJ7">
-        <v>1.86415826941827E-06</v>
+        <v>0</v>
       </c>
       <c r="DK7">
-        <v>0.00455591723235476</v>
+        <v>0</v>
       </c>
       <c r="DL7">
-        <v>0.006007758747740272</v>
+        <v>0</v>
       </c>
       <c r="DM7">
-        <v>1.063819396663898E-05</v>
+        <v>0</v>
       </c>
       <c r="DN7">
         <v>0</v>
@@ -3587,100 +3587,100 @@
         <v>0</v>
       </c>
       <c r="CH8">
-        <v>0.198081402365918</v>
+        <v>0.317780110200292</v>
       </c>
       <c r="CI8">
-        <v>0.004275706466927469</v>
+        <v>0</v>
       </c>
       <c r="CJ8">
-        <v>0.1934919918114391</v>
+        <v>0.3091032228633953</v>
       </c>
       <c r="CK8">
-        <v>0.01686852772817523</v>
+        <v>0</v>
       </c>
       <c r="CL8">
-        <v>0.006590067771226634</v>
+        <v>0</v>
       </c>
       <c r="CM8">
-        <v>0.05839702573721122</v>
+        <v>0.05368833101764572</v>
       </c>
       <c r="CN8">
-        <v>0.0374291362228065</v>
+        <v>0.01404576410206781</v>
       </c>
       <c r="CO8">
-        <v>0.02258294158335281</v>
+        <v>0</v>
       </c>
       <c r="CP8">
-        <v>0.0007036054836352561</v>
+        <v>0</v>
       </c>
       <c r="CQ8">
-        <v>0.02265979853463983</v>
+        <v>0</v>
       </c>
       <c r="CR8">
-        <v>0.01729803091249707</v>
+        <v>0</v>
       </c>
       <c r="CS8">
-        <v>0.08092237989986947</v>
+        <v>0.09627549073521362</v>
       </c>
       <c r="CT8">
-        <v>0.04623434684471471</v>
+        <v>0.03069317876175267</v>
       </c>
       <c r="CU8">
-        <v>0.02671116066661588</v>
+        <v>0</v>
       </c>
       <c r="CV8">
-        <v>0.0249107451131393</v>
+        <v>0</v>
       </c>
       <c r="CW8">
-        <v>0.1031214873628684</v>
+        <v>0.138245837939851</v>
       </c>
       <c r="CX8">
-        <v>0.0006169866489721357</v>
+        <v>0</v>
       </c>
       <c r="CY8">
-        <v>0.05124583752904758</v>
+        <v>0.04016806437978199</v>
       </c>
       <c r="CZ8">
-        <v>0.001199490293247548</v>
+        <v>0</v>
       </c>
       <c r="DA8">
-        <v>0.0002152097591175756</v>
+        <v>0</v>
       </c>
       <c r="DB8">
-        <v>0.01764720393013972</v>
+        <v>0</v>
       </c>
       <c r="DC8">
-        <v>0.0002446395464405495</v>
+        <v>0</v>
       </c>
       <c r="DD8">
-        <v>0.01046016001895371</v>
+        <v>0</v>
       </c>
       <c r="DE8">
-        <v>0.005155446242268155</v>
+        <v>0</v>
       </c>
       <c r="DF8">
-        <v>0.008042341793698161</v>
+        <v>0</v>
       </c>
       <c r="DG8">
-        <v>0.005112826021677111</v>
+        <v>0</v>
       </c>
       <c r="DH8">
-        <v>0.01531746791801691</v>
+        <v>0</v>
       </c>
       <c r="DI8">
-        <v>0.00747528236025918</v>
+        <v>0</v>
       </c>
       <c r="DJ8">
-        <v>0.0008255348898943177</v>
+        <v>0</v>
       </c>
       <c r="DK8">
-        <v>0.01037510840258359</v>
+        <v>0</v>
       </c>
       <c r="DL8">
-        <v>0.005768379599390617</v>
+        <v>0</v>
       </c>
       <c r="DM8">
-        <v>1.973054125632185E-05</v>
+        <v>0</v>
       </c>
       <c r="DN8">
         <v>0</v>
@@ -3832,100 +3832,100 @@
         <v>0</v>
       </c>
       <c r="AV9">
-        <v>0.05059154123310714</v>
+        <v>0.04380071559665513</v>
       </c>
       <c r="AW9">
-        <v>0.1100674843873066</v>
+        <v>0.1703132889610737</v>
       </c>
       <c r="AX9">
-        <v>0.1846234502978343</v>
+        <v>0.328902906994642</v>
       </c>
       <c r="AY9">
-        <v>0.05572003142312925</v>
+        <v>0.05470963871758357</v>
       </c>
       <c r="AZ9">
-        <v>0.005287254379638884</v>
+        <v>0</v>
       </c>
       <c r="BA9">
-        <v>0.01818882998534225</v>
+        <v>0</v>
       </c>
       <c r="BB9">
-        <v>0.05093977113935689</v>
+        <v>0.04454144301055903</v>
       </c>
       <c r="BC9">
-        <v>0.00323001095478042</v>
+        <v>0</v>
       </c>
       <c r="BD9">
-        <v>0.01088811197514997</v>
+        <v>0</v>
       </c>
       <c r="BE9">
-        <v>0.02073495949203113</v>
+        <v>0</v>
       </c>
       <c r="BF9">
-        <v>0.02083752163738676</v>
+        <v>0</v>
       </c>
       <c r="BG9">
-        <v>0.05681884362381847</v>
+        <v>0.057046946068776</v>
       </c>
       <c r="BH9">
-        <v>0.1173771122826847</v>
+        <v>0.1858617575743928</v>
       </c>
       <c r="BI9">
-        <v>0.0005994637995832678</v>
+        <v>0</v>
       </c>
       <c r="BJ9">
-        <v>0.03798717808821047</v>
+        <v>0.0169897003775056</v>
       </c>
       <c r="BK9">
-        <v>0.02639768722254921</v>
+        <v>0</v>
       </c>
       <c r="BL9">
-        <v>0.06868910485839307</v>
+        <v>0.08229643713444054</v>
       </c>
       <c r="BM9">
-        <v>0.03730431411921496</v>
+        <v>0.01553716556437144</v>
       </c>
       <c r="BN9">
-        <v>0.001834871306532972</v>
+        <v>0</v>
       </c>
       <c r="BO9">
-        <v>0.007956842224582305</v>
+        <v>0</v>
       </c>
       <c r="BP9">
-        <v>0.005998475634110493</v>
+        <v>0</v>
       </c>
       <c r="BQ9">
-        <v>0.007239940676348388</v>
+        <v>0</v>
       </c>
       <c r="BR9">
-        <v>0.003610876776551087</v>
+        <v>0</v>
       </c>
       <c r="BS9">
-        <v>0.003501475050870057</v>
+        <v>0</v>
       </c>
       <c r="BT9">
-        <v>0.001560497169733459</v>
+        <v>0</v>
       </c>
       <c r="BU9">
-        <v>0.01191646480042355</v>
+        <v>0</v>
       </c>
       <c r="BV9">
-        <v>0.02021145892283963</v>
+        <v>0</v>
       </c>
       <c r="BW9">
-        <v>0.02607794925575022</v>
+        <v>0</v>
       </c>
       <c r="BX9">
-        <v>0.004992021753053369</v>
+        <v>0</v>
       </c>
       <c r="BY9">
-        <v>0.01012181556186766</v>
+        <v>0</v>
       </c>
       <c r="BZ9">
-        <v>0.01674908906938557</v>
+        <v>0</v>
       </c>
       <c r="CA9">
-        <v>0.001945550898433526</v>
+        <v>0</v>
       </c>
       <c r="CB9">
         <v>0</v>
@@ -4059,13 +4059,13 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.05644232829206049</v>
+        <v>0.05117150718014198</v>
       </c>
       <c r="E10">
-        <v>0.09467701459934753</v>
+        <v>0.1239108651785945</v>
       </c>
       <c r="F10">
-        <v>0.003669866939727705</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -4074,22 +4074,22 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.007304816395099724</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>0.02826572764390175</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>0.004304138299309938</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>0.03103977458490679</v>
+        <v>0.002844565687034677</v>
       </c>
       <c r="M10">
-        <v>0.04713893059754778</v>
+        <v>0.03347231200264254</v>
       </c>
       <c r="N10">
-        <v>5.040408960125007E-05</v>
+        <v>0</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -4101,58 +4101,58 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>0.01474426401225366</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>0.02877092040651047</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <v>0.06810655340400486</v>
+        <v>0.07336204483418199</v>
       </c>
       <c r="U10">
-        <v>0.01444418594018261</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <v>0.01532609011181746</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>0.1213548001516441</v>
+        <v>0.1746638641256424</v>
       </c>
       <c r="X10">
-        <v>0.1574168608086315</v>
+        <v>0.2432699230117744</v>
       </c>
       <c r="Y10">
-        <v>0.1400691554302283</v>
+        <v>0.2102668811709196</v>
       </c>
       <c r="Z10">
-        <v>0.05891621135983128</v>
+        <v>0.05587793172529624</v>
       </c>
       <c r="AA10">
-        <v>0.01149010348393166</v>
+        <v>0</v>
       </c>
       <c r="AB10">
-        <v>0.004251762577489132</v>
+        <v>0</v>
       </c>
       <c r="AC10">
         <v>0</v>
       </c>
       <c r="AD10">
-        <v>0.002366976837269733</v>
+        <v>0</v>
       </c>
       <c r="AE10">
-        <v>0.006597604513331674</v>
+        <v>0</v>
       </c>
       <c r="AF10">
-        <v>0.002118927917615176</v>
+        <v>0</v>
       </c>
       <c r="AG10">
-        <v>0.01350703871765859</v>
+        <v>0</v>
       </c>
       <c r="AH10">
-        <v>0.02170199978512899</v>
+        <v>0</v>
       </c>
       <c r="AI10">
-        <v>0.04592354310096787</v>
+        <v>0.0311601050837716</v>
       </c>
       <c r="AJ10">
         <v>0</v>
@@ -4670,100 +4670,100 @@
         <v>0</v>
       </c>
       <c r="CJ11">
-        <v>0.2617457971327486</v>
+        <v>0.4217467650485255</v>
       </c>
       <c r="CK11">
-        <v>0.02072714234559451</v>
+        <v>0</v>
       </c>
       <c r="CL11">
-        <v>0.1895715914300729</v>
+        <v>0.2903992361972725</v>
       </c>
       <c r="CM11">
-        <v>0.03481669400221733</v>
+        <v>0.008765747378366259</v>
       </c>
       <c r="CN11">
-        <v>0.02796351029202453</v>
+        <v>0</v>
       </c>
       <c r="CO11">
-        <v>0.02436487501259955</v>
+        <v>0</v>
       </c>
       <c r="CP11">
-        <v>0.01436690785828741</v>
+        <v>0</v>
       </c>
       <c r="CQ11">
-        <v>0.009898095935438309</v>
+        <v>0</v>
       </c>
       <c r="CR11">
-        <v>0.0005388689754388296</v>
+        <v>0</v>
       </c>
       <c r="CS11">
-        <v>0.005761496737508212</v>
+        <v>0</v>
       </c>
       <c r="CT11">
-        <v>0.03924866323684714</v>
+        <v>0.01683134645556988</v>
       </c>
       <c r="CU11">
-        <v>0.1017147401970358</v>
+        <v>0.1305113622710927</v>
       </c>
       <c r="CV11">
-        <v>0.01005816936779222</v>
+        <v>0</v>
       </c>
       <c r="CW11">
-        <v>0.0486536908738668</v>
+        <v>0.03394725548253232</v>
       </c>
       <c r="CX11">
-        <v>0.01372697411824402</v>
+        <v>0</v>
       </c>
       <c r="CY11">
-        <v>0.05609863301572932</v>
+        <v>0.04749606759973922</v>
       </c>
       <c r="CZ11">
-        <v>0.01334196203113425</v>
+        <v>0</v>
       </c>
       <c r="DA11">
-        <v>0.05764058657269579</v>
+        <v>0.05030221956690162</v>
       </c>
       <c r="DB11">
-        <v>3.860252651799622E-05</v>
+        <v>0</v>
       </c>
       <c r="DC11">
-        <v>0.0008383843049554961</v>
+        <v>0</v>
       </c>
       <c r="DD11">
-        <v>0.01110280299437544</v>
+        <v>0</v>
       </c>
       <c r="DE11">
-        <v>0.002581093408670482</v>
+        <v>0</v>
       </c>
       <c r="DF11">
-        <v>0.01567040008988011</v>
+        <v>0</v>
       </c>
       <c r="DG11">
-        <v>0.01111525066986863</v>
+        <v>0</v>
       </c>
       <c r="DH11">
-        <v>0.0003659886794237279</v>
+        <v>0</v>
       </c>
       <c r="DI11">
-        <v>0.001869527999785427</v>
+        <v>0</v>
       </c>
       <c r="DJ11">
-        <v>0.01369434023900183</v>
+        <v>0</v>
       </c>
       <c r="DK11">
-        <v>0.004439701961061493</v>
+        <v>0</v>
       </c>
       <c r="DL11">
-        <v>0.0008454600438758443</v>
+        <v>0</v>
       </c>
       <c r="DM11">
-        <v>0.003871851741447134</v>
+        <v>0</v>
       </c>
       <c r="DN11">
-        <v>0.002795286808893945</v>
+        <v>0</v>
       </c>
       <c r="DO11">
-        <v>0.0005329093969666564</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5395,106 +5395,106 @@
         <v>0</v>
       </c>
       <c r="CH2">
-        <v>0.2249777582959693</v>
+        <v>0.3047491211860124</v>
       </c>
       <c r="CI2">
-        <v>0.4945540160456422</v>
+        <v>0.6792054419701443</v>
       </c>
       <c r="CJ2">
-        <v>0.596791837741518</v>
+        <v>0.7921127441701877</v>
       </c>
       <c r="CK2">
-        <v>0.6060965009447933</v>
+        <v>0.7921127441701877</v>
       </c>
       <c r="CL2">
-        <v>0.6435529006681757</v>
+        <v>0.8037670542964901</v>
       </c>
       <c r="CM2">
-        <v>0.6464107235358506</v>
+        <v>0.8037670542964901</v>
       </c>
       <c r="CN2">
-        <v>0.6513362094553584</v>
+        <v>0.8037670542964901</v>
       </c>
       <c r="CO2">
-        <v>0.6564190819534125</v>
+        <v>0.8037670542964901</v>
       </c>
       <c r="CP2">
-        <v>0.6681827523307784</v>
+        <v>0.8037670542964901</v>
       </c>
       <c r="CQ2">
-        <v>0.6681963875218829</v>
+        <v>0.8037670542964901</v>
       </c>
       <c r="CR2">
-        <v>0.6795900556243498</v>
+        <v>0.8037670542964901</v>
       </c>
       <c r="CS2">
-        <v>0.8143637124523496</v>
+        <v>0.9675276807434803</v>
       </c>
       <c r="CT2">
-        <v>0.8145393491975141</v>
+        <v>0.9675276807434803</v>
       </c>
       <c r="CU2">
-        <v>0.8653150613330143</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="CV2">
-        <v>0.8724144076614189</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="CW2">
-        <v>0.886209818161878</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="CX2">
-        <v>0.9106504043751427</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="CY2">
-        <v>0.9106588220181923</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="CZ2">
-        <v>0.9164407297522597</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DA2">
-        <v>0.9304360488468972</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DB2">
-        <v>0.9305006605245574</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DC2">
-        <v>0.9573620955669377</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DD2">
-        <v>0.9600353747636616</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DE2">
-        <v>0.9656150768952828</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DF2">
-        <v>0.9672720029699751</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DG2">
-        <v>0.9805394372037868</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DH2">
-        <v>0.9893230807107933</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DI2">
-        <v>0.9899075419276595</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DJ2">
-        <v>0.990088222259177</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DK2">
-        <v>0.9939790423512329</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DL2">
-        <v>0.9997951347037699</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DM2">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DN2">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="DO2">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:119">
@@ -5754,97 +5754,97 @@
         <v>0</v>
       </c>
       <c r="CH3">
-        <v>0.1479818478787089</v>
+        <v>0.208813990958931</v>
       </c>
       <c r="CI3">
-        <v>0.4130575313292739</v>
+        <v>0.6256156386369657</v>
       </c>
       <c r="CJ3">
-        <v>0.4896475872716364</v>
+        <v>0.707620123004011</v>
       </c>
       <c r="CK3">
-        <v>0.5033074694108111</v>
+        <v>0.707620123004011</v>
       </c>
       <c r="CL3">
-        <v>0.5265198359728273</v>
+        <v>0.707620123004011</v>
       </c>
       <c r="CM3">
-        <v>0.5298768007816999</v>
+        <v>0.707620123004011</v>
       </c>
       <c r="CN3">
-        <v>0.5545283398302185</v>
+        <v>0.707620123004011</v>
       </c>
       <c r="CO3">
-        <v>0.5650741229293228</v>
+        <v>0.707620123004011</v>
       </c>
       <c r="CP3">
-        <v>0.5890526971042148</v>
+        <v>0.707620123004011</v>
       </c>
       <c r="CQ3">
-        <v>0.5901524386967536</v>
+        <v>0.707620123004011</v>
       </c>
       <c r="CR3">
-        <v>0.6147892472182865</v>
+        <v>0.707620123004011</v>
       </c>
       <c r="CS3">
-        <v>0.7576194513916251</v>
+        <v>0.9072835186536428</v>
       </c>
       <c r="CT3">
-        <v>0.7647080787946177</v>
+        <v>0.9072835186536428</v>
       </c>
       <c r="CU3">
-        <v>0.8302273868702849</v>
+        <v>0.9696236125284237</v>
       </c>
       <c r="CV3">
-        <v>0.8501468798849484</v>
+        <v>0.9696236125284237</v>
       </c>
       <c r="CW3">
-        <v>0.8565086767895899</v>
+        <v>0.9696236125284237</v>
       </c>
       <c r="CX3">
-        <v>0.90403291226872</v>
+        <v>1</v>
       </c>
       <c r="CY3">
-        <v>0.9043070056429939</v>
+        <v>1</v>
       </c>
       <c r="CZ3">
-        <v>0.9102325369320728</v>
+        <v>1</v>
       </c>
       <c r="DA3">
-        <v>0.9280792395559316</v>
+        <v>1</v>
       </c>
       <c r="DB3">
-        <v>0.928135870423403</v>
+        <v>1</v>
       </c>
       <c r="DC3">
-        <v>0.9543837453501868</v>
+        <v>1</v>
       </c>
       <c r="DD3">
-        <v>0.9592557923221939</v>
+        <v>1</v>
       </c>
       <c r="DE3">
-        <v>0.9599647388704261</v>
+        <v>1</v>
       </c>
       <c r="DF3">
-        <v>0.9620243316497529</v>
+        <v>1</v>
       </c>
       <c r="DG3">
-        <v>0.9781554474034441</v>
+        <v>1</v>
       </c>
       <c r="DH3">
-        <v>0.9890639997678735</v>
+        <v>1</v>
       </c>
       <c r="DI3">
-        <v>0.9891414357323454</v>
+        <v>1</v>
       </c>
       <c r="DJ3">
-        <v>0.9906383567164156</v>
+        <v>1</v>
       </c>
       <c r="DK3">
-        <v>0.9950222979490453</v>
+        <v>1</v>
       </c>
       <c r="DL3">
-        <v>0.997812883188535</v>
+        <v>1</v>
       </c>
       <c r="DM3">
         <v>1</v>
@@ -6116,103 +6116,103 @@
         <v>0</v>
       </c>
       <c r="CI4">
-        <v>0.1196721865236701</v>
+        <v>0.1671051085991076</v>
       </c>
       <c r="CJ4">
-        <v>0.1234629700227281</v>
+        <v>0.1671051085991076</v>
       </c>
       <c r="CK4">
-        <v>0.3745739030257618</v>
+        <v>0.5791477709263932</v>
       </c>
       <c r="CL4">
-        <v>0.38522211932303</v>
+        <v>0.5791477709263932</v>
       </c>
       <c r="CM4">
-        <v>0.3954793298857723</v>
+        <v>0.5791477709263932</v>
       </c>
       <c r="CN4">
-        <v>0.423713954661739</v>
+        <v>0.5791477709263932</v>
       </c>
       <c r="CO4">
-        <v>0.4307319314278081</v>
+        <v>0.5791477709263932</v>
       </c>
       <c r="CP4">
-        <v>0.4471987407531126</v>
+        <v>0.5791477709263932</v>
       </c>
       <c r="CQ4">
-        <v>0.4472547846074042</v>
+        <v>0.5791477709263932</v>
       </c>
       <c r="CR4">
-        <v>0.4899106411668127</v>
+        <v>0.6027320992087916</v>
       </c>
       <c r="CS4">
-        <v>0.4899721126562827</v>
+        <v>0.6027320992087916</v>
       </c>
       <c r="CT4">
-        <v>0.5935404464725584</v>
+        <v>0.7398275006750992</v>
       </c>
       <c r="CU4">
-        <v>0.7109084531338365</v>
+        <v>0.9026387446873847</v>
       </c>
       <c r="CV4">
-        <v>0.7487329525366648</v>
+        <v>0.9172197856225037</v>
       </c>
       <c r="CW4">
-        <v>0.7714318341212829</v>
+        <v>0.9172197856225037</v>
       </c>
       <c r="CX4">
-        <v>0.8350982804078538</v>
+        <v>0.9799575795914113</v>
       </c>
       <c r="CY4">
-        <v>0.8352826235073261</v>
+        <v>0.9799575795914113</v>
       </c>
       <c r="CZ4">
-        <v>0.8701241754037894</v>
+        <v>0.9889798649489024</v>
       </c>
       <c r="DA4">
-        <v>0.876738720774722</v>
+        <v>0.9889798649489024</v>
       </c>
       <c r="DB4">
-        <v>0.876914980616332</v>
+        <v>0.9889798649489024</v>
       </c>
       <c r="DC4">
-        <v>0.9075427803747935</v>
+        <v>0.990149776722923</v>
       </c>
       <c r="DD4">
-        <v>0.909646252059508</v>
+        <v>0.990149776722923</v>
       </c>
       <c r="DE4">
-        <v>0.9179719989927615</v>
+        <v>0.990149776722923</v>
       </c>
       <c r="DF4">
-        <v>0.9184770461055256</v>
+        <v>0.990149776722923</v>
       </c>
       <c r="DG4">
-        <v>0.922530807459612</v>
+        <v>0.990149776722923</v>
       </c>
       <c r="DH4">
-        <v>0.944159526658391</v>
+        <v>0.990149776722923</v>
       </c>
       <c r="DI4">
-        <v>0.9794453678059579</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="DJ4">
-        <v>0.9855671243330087</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="DK4">
-        <v>0.9867226460112584</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="DL4">
-        <v>0.9935245280596047</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="DM4">
-        <v>0.9994784333918144</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="DN4">
-        <v>1</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="DO4">
-        <v>1</v>
+        <v>0.9999999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:119">
@@ -6475,97 +6475,97 @@
         <v>0</v>
       </c>
       <c r="CI5">
-        <v>0.1681583925085048</v>
+        <v>0.2609878969724378</v>
       </c>
       <c r="CJ5">
-        <v>0.1715401089298946</v>
+        <v>0.2609878969724378</v>
       </c>
       <c r="CK5">
-        <v>0.4209912278218294</v>
+        <v>0.6755416925685236</v>
       </c>
       <c r="CL5">
-        <v>0.4389947919682559</v>
+        <v>0.6755416925685236</v>
       </c>
       <c r="CM5">
-        <v>0.478303288763446</v>
+        <v>0.693125893994447</v>
       </c>
       <c r="CN5">
-        <v>0.5112661015894928</v>
+        <v>0.6987227909657645</v>
       </c>
       <c r="CO5">
-        <v>0.5112697023056428</v>
+        <v>0.6987227909657645</v>
       </c>
       <c r="CP5">
-        <v>0.5220743121209661</v>
+        <v>0.6987227909657645</v>
       </c>
       <c r="CQ5">
-        <v>0.5361187330652557</v>
+        <v>0.6987227909657645</v>
       </c>
       <c r="CR5">
-        <v>0.55411242562772</v>
+        <v>0.6987227909657645</v>
       </c>
       <c r="CS5">
-        <v>0.5546159454378217</v>
+        <v>0.6987227909657645</v>
       </c>
       <c r="CT5">
-        <v>0.6303352516728519</v>
+        <v>0.7850887754613128</v>
       </c>
       <c r="CU5">
-        <v>0.7033332573165157</v>
+        <v>0.8663140912976856</v>
       </c>
       <c r="CV5">
-        <v>0.7477619868649547</v>
+        <v>0.8935706604604986</v>
       </c>
       <c r="CW5">
-        <v>0.7622170608315877</v>
+        <v>0.8935706604604986</v>
       </c>
       <c r="CX5">
-        <v>0.8485572460934055</v>
+        <v>1</v>
       </c>
       <c r="CY5">
-        <v>0.8503853915592965</v>
+        <v>1</v>
       </c>
       <c r="CZ5">
-        <v>0.8675221580193664</v>
+        <v>1</v>
       </c>
       <c r="DA5">
-        <v>0.8910857661961618</v>
+        <v>1</v>
       </c>
       <c r="DB5">
-        <v>0.8915472771807349</v>
+        <v>1</v>
       </c>
       <c r="DC5">
-        <v>0.910867452492105</v>
+        <v>1</v>
       </c>
       <c r="DD5">
-        <v>0.9252441687962409</v>
+        <v>1</v>
       </c>
       <c r="DE5">
-        <v>0.9443181854575203</v>
+        <v>1</v>
       </c>
       <c r="DF5">
-        <v>0.9481641397363502</v>
+        <v>1</v>
       </c>
       <c r="DG5">
-        <v>0.9487786579035111</v>
+        <v>1</v>
       </c>
       <c r="DH5">
-        <v>0.9551736659204682</v>
+        <v>1</v>
       </c>
       <c r="DI5">
-        <v>0.9838227847328037</v>
+        <v>1</v>
       </c>
       <c r="DJ5">
-        <v>0.9883106370430359</v>
+        <v>1</v>
       </c>
       <c r="DK5">
-        <v>0.9883139938447217</v>
+        <v>1</v>
       </c>
       <c r="DL5">
-        <v>0.9917693953641075</v>
+        <v>1</v>
       </c>
       <c r="DM5">
-        <v>0.9993328965094552</v>
+        <v>1</v>
       </c>
       <c r="DN5">
         <v>1</v>
@@ -6831,97 +6831,97 @@
         <v>0</v>
       </c>
       <c r="CH6">
-        <v>0.2303706899218832</v>
+        <v>0.3505469830983896</v>
       </c>
       <c r="CI6">
-        <v>0.2709352030469159</v>
+        <v>0.3690295176713222</v>
       </c>
       <c r="CJ6">
-        <v>0.3793583495948656</v>
+        <v>0.506230210238605</v>
       </c>
       <c r="CK6">
-        <v>0.3794790406406877</v>
+        <v>0.506230210238605</v>
       </c>
       <c r="CL6">
-        <v>0.4168713475557017</v>
+        <v>0.51916299441081</v>
       </c>
       <c r="CM6">
-        <v>0.4503790909419609</v>
+        <v>0.5252997645243226</v>
       </c>
       <c r="CN6">
-        <v>0.4755692349136042</v>
+        <v>0.5252997645243226</v>
       </c>
       <c r="CO6">
-        <v>0.4790159227392782</v>
+        <v>0.5252997645243226</v>
       </c>
       <c r="CP6">
-        <v>0.4805505857847734</v>
+        <v>0.5252997645243226</v>
       </c>
       <c r="CQ6">
-        <v>0.4994322052580136</v>
+        <v>0.5252997645243226</v>
       </c>
       <c r="CR6">
-        <v>0.4999232808851315</v>
+        <v>0.5252997645243226</v>
       </c>
       <c r="CS6">
-        <v>0.6210275634083369</v>
+        <v>0.6846860070845679</v>
       </c>
       <c r="CT6">
-        <v>0.6582618357884465</v>
+        <v>0.6973423110517206</v>
       </c>
       <c r="CU6">
-        <v>0.7705380677611648</v>
+        <v>0.8412839469765355</v>
       </c>
       <c r="CV6">
-        <v>0.7705382865874651</v>
+        <v>0.8412839469765355</v>
       </c>
       <c r="CW6">
-        <v>0.8912594925293911</v>
+        <v>1</v>
       </c>
       <c r="CX6">
-        <v>0.9199374231532217</v>
+        <v>1</v>
       </c>
       <c r="CY6">
-        <v>0.9351532504227013</v>
+        <v>1</v>
       </c>
       <c r="CZ6">
-        <v>0.9456957324863624</v>
+        <v>1</v>
       </c>
       <c r="DA6">
-        <v>0.951570414799886</v>
+        <v>1</v>
       </c>
       <c r="DB6">
-        <v>0.9583197991870338</v>
+        <v>1</v>
       </c>
       <c r="DC6">
-        <v>0.9671119234370871</v>
+        <v>1</v>
       </c>
       <c r="DD6">
-        <v>0.9676152811037265</v>
+        <v>1</v>
       </c>
       <c r="DE6">
-        <v>0.9695873098074204</v>
+        <v>1</v>
       </c>
       <c r="DF6">
-        <v>0.9748575408215812</v>
+        <v>1</v>
       </c>
       <c r="DG6">
-        <v>0.9773345824788896</v>
+        <v>1</v>
       </c>
       <c r="DH6">
-        <v>0.9902578987873725</v>
+        <v>1</v>
       </c>
       <c r="DI6">
-        <v>0.9915973783425902</v>
+        <v>1</v>
       </c>
       <c r="DJ6">
-        <v>0.9928782219819142</v>
+        <v>1</v>
       </c>
       <c r="DK6">
-        <v>0.9974291826259069</v>
+        <v>1</v>
       </c>
       <c r="DL6">
-        <v>0.9975314174044885</v>
+        <v>1</v>
       </c>
       <c r="DM6">
         <v>1</v>
@@ -7190,97 +7190,97 @@
         <v>0</v>
       </c>
       <c r="CH7">
-        <v>0.2532391155057309</v>
+        <v>0.3918612947215527</v>
       </c>
       <c r="CI7">
-        <v>0.2977124632922515</v>
+        <v>0.4172669893720303</v>
       </c>
       <c r="CJ7">
-        <v>0.4882936859617672</v>
+        <v>0.6991421691795358</v>
       </c>
       <c r="CK7">
-        <v>0.4987052959150279</v>
+        <v>0.6991421691795358</v>
       </c>
       <c r="CL7">
-        <v>0.5089502041521814</v>
+        <v>0.6991421691795358</v>
       </c>
       <c r="CM7">
-        <v>0.571299225556429</v>
+        <v>0.7559258084701969</v>
       </c>
       <c r="CN7">
-        <v>0.5740752661499329</v>
+        <v>0.7559258084701969</v>
       </c>
       <c r="CO7">
-        <v>0.5815214135882567</v>
+        <v>0.7559258084701969</v>
       </c>
       <c r="CP7">
-        <v>0.5817574329197072</v>
+        <v>0.7559258084701969</v>
       </c>
       <c r="CQ7">
-        <v>0.6058878384267518</v>
+        <v>0.7559258084701969</v>
       </c>
       <c r="CR7">
-        <v>0.6199250297114872</v>
+        <v>0.7559258084701969</v>
       </c>
       <c r="CS7">
-        <v>0.7304060613318696</v>
+        <v>0.8971976513541992</v>
       </c>
       <c r="CT7">
-        <v>0.7441405526729655</v>
+        <v>0.8971976513541992</v>
       </c>
       <c r="CU7">
-        <v>0.7925004629289261</v>
+        <v>0.9294255975524877</v>
       </c>
       <c r="CV7">
-        <v>0.7966701087017773</v>
+        <v>0.9294255975524877</v>
       </c>
       <c r="CW7">
-        <v>0.8668755778102364</v>
+        <v>1</v>
       </c>
       <c r="CX7">
-        <v>0.8831577604689748</v>
+        <v>1</v>
       </c>
       <c r="CY7">
-        <v>0.9078030919533135</v>
+        <v>1</v>
       </c>
       <c r="CZ7">
-        <v>0.9110008236069759</v>
+        <v>1</v>
       </c>
       <c r="DA7">
-        <v>0.9120197713035333</v>
+        <v>1</v>
       </c>
       <c r="DB7">
-        <v>0.9334492385817339</v>
+        <v>1</v>
       </c>
       <c r="DC7">
-        <v>0.940224839234692</v>
+        <v>1</v>
       </c>
       <c r="DD7">
-        <v>0.9553798329892984</v>
+        <v>1</v>
       </c>
       <c r="DE7">
-        <v>0.9578800978522392</v>
+        <v>1</v>
       </c>
       <c r="DF7">
-        <v>0.9612328733612462</v>
+        <v>1</v>
       </c>
       <c r="DG7">
-        <v>0.9641409007396203</v>
+        <v>1</v>
       </c>
       <c r="DH7">
-        <v>0.9864907053848715</v>
+        <v>1</v>
       </c>
       <c r="DI7">
-        <v>0.989423821667669</v>
+        <v>1</v>
       </c>
       <c r="DJ7">
-        <v>0.9894256858259384</v>
+        <v>1</v>
       </c>
       <c r="DK7">
-        <v>0.9939816030582931</v>
+        <v>1</v>
       </c>
       <c r="DL7">
-        <v>0.9999893618060334</v>
+        <v>1</v>
       </c>
       <c r="DM7">
         <v>1</v>
@@ -7549,106 +7549,106 @@
         <v>0</v>
       </c>
       <c r="CH8">
-        <v>0.198081402365918</v>
+        <v>0.317780110200292</v>
       </c>
       <c r="CI8">
-        <v>0.2023571088328455</v>
+        <v>0.317780110200292</v>
       </c>
       <c r="CJ8">
-        <v>0.3958491006442846</v>
+        <v>0.6268833330636873</v>
       </c>
       <c r="CK8">
-        <v>0.4127176283724598</v>
+        <v>0.6268833330636873</v>
       </c>
       <c r="CL8">
-        <v>0.4193076961436864</v>
+        <v>0.6268833330636873</v>
       </c>
       <c r="CM8">
-        <v>0.4777047218808976</v>
+        <v>0.680571664081333</v>
       </c>
       <c r="CN8">
-        <v>0.5151338581037042</v>
+        <v>0.6946174281834008</v>
       </c>
       <c r="CO8">
-        <v>0.537716799687057</v>
+        <v>0.6946174281834008</v>
       </c>
       <c r="CP8">
-        <v>0.5384204051706922</v>
+        <v>0.6946174281834008</v>
       </c>
       <c r="CQ8">
-        <v>0.5610802037053321</v>
+        <v>0.6946174281834008</v>
       </c>
       <c r="CR8">
-        <v>0.5783782346178291</v>
+        <v>0.6946174281834008</v>
       </c>
       <c r="CS8">
-        <v>0.6593006145176986</v>
+        <v>0.7908929189186144</v>
       </c>
       <c r="CT8">
-        <v>0.7055349613624133</v>
+        <v>0.8215860976803671</v>
       </c>
       <c r="CU8">
-        <v>0.7322461220290292</v>
+        <v>0.8215860976803671</v>
       </c>
       <c r="CV8">
-        <v>0.7571568671421685</v>
+        <v>0.8215860976803671</v>
       </c>
       <c r="CW8">
-        <v>0.8602783545050369</v>
+        <v>0.9598319356202181</v>
       </c>
       <c r="CX8">
-        <v>0.860895341154009</v>
+        <v>0.9598319356202181</v>
       </c>
       <c r="CY8">
-        <v>0.9121411786830566</v>
+        <v>1</v>
       </c>
       <c r="CZ8">
-        <v>0.9133406689763041</v>
+        <v>1</v>
       </c>
       <c r="DA8">
-        <v>0.9135558787354217</v>
+        <v>1</v>
       </c>
       <c r="DB8">
-        <v>0.9312030826655614</v>
+        <v>1</v>
       </c>
       <c r="DC8">
-        <v>0.9314477222120019</v>
+        <v>1</v>
       </c>
       <c r="DD8">
-        <v>0.9419078822309556</v>
+        <v>1</v>
       </c>
       <c r="DE8">
-        <v>0.9470633284732237</v>
+        <v>1</v>
       </c>
       <c r="DF8">
-        <v>0.9551056702669218</v>
+        <v>1</v>
       </c>
       <c r="DG8">
-        <v>0.9602184962885989</v>
+        <v>1</v>
       </c>
       <c r="DH8">
-        <v>0.9755359642066158</v>
+        <v>1</v>
       </c>
       <c r="DI8">
-        <v>0.983011246566875</v>
+        <v>1</v>
       </c>
       <c r="DJ8">
-        <v>0.9838367814567693</v>
+        <v>1</v>
       </c>
       <c r="DK8">
-        <v>0.9942118898593529</v>
+        <v>1</v>
       </c>
       <c r="DL8">
-        <v>0.9999802694587435</v>
+        <v>1</v>
       </c>
       <c r="DM8">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="DN8">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="DO8">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:119">
@@ -7794,97 +7794,97 @@
         <v>0</v>
       </c>
       <c r="AV9">
-        <v>0.05059154123310714</v>
+        <v>0.04380071559665513</v>
       </c>
       <c r="AW9">
-        <v>0.1606590256204138</v>
+        <v>0.2141140045577289</v>
       </c>
       <c r="AX9">
-        <v>0.3452824759182481</v>
+        <v>0.5430169115523709</v>
       </c>
       <c r="AY9">
-        <v>0.4010025073413773</v>
+        <v>0.5977265502699545</v>
       </c>
       <c r="AZ9">
-        <v>0.4062897617210162</v>
+        <v>0.5977265502699545</v>
       </c>
       <c r="BA9">
-        <v>0.4244785917063585</v>
+        <v>0.5977265502699545</v>
       </c>
       <c r="BB9">
-        <v>0.4754183628457154</v>
+        <v>0.6422679932805135</v>
       </c>
       <c r="BC9">
-        <v>0.4786483738004958</v>
+        <v>0.6422679932805135</v>
       </c>
       <c r="BD9">
-        <v>0.4895364857756458</v>
+        <v>0.6422679932805135</v>
       </c>
       <c r="BE9">
-        <v>0.5102714452676769</v>
+        <v>0.6422679932805135</v>
       </c>
       <c r="BF9">
-        <v>0.5311089669050636</v>
+        <v>0.6422679932805135</v>
       </c>
       <c r="BG9">
-        <v>0.5879278105288821</v>
+        <v>0.6993149393492896</v>
       </c>
       <c r="BH9">
-        <v>0.7053049228115669</v>
+        <v>0.8851766969236824</v>
       </c>
       <c r="BI9">
-        <v>0.7059043866111502</v>
+        <v>0.8851766969236824</v>
       </c>
       <c r="BJ9">
-        <v>0.7438915646993607</v>
+        <v>0.902166397301188</v>
       </c>
       <c r="BK9">
-        <v>0.7702892519219099</v>
+        <v>0.902166397301188</v>
       </c>
       <c r="BL9">
-        <v>0.838978356780303</v>
+        <v>0.9844628344356285</v>
       </c>
       <c r="BM9">
-        <v>0.8762826708995179</v>
+        <v>1</v>
       </c>
       <c r="BN9">
-        <v>0.8781175422060509</v>
+        <v>1</v>
       </c>
       <c r="BO9">
-        <v>0.8860743844306331</v>
+        <v>1</v>
       </c>
       <c r="BP9">
-        <v>0.8920728600647436</v>
+        <v>1</v>
       </c>
       <c r="BQ9">
-        <v>0.899312800741092</v>
+        <v>1</v>
       </c>
       <c r="BR9">
-        <v>0.9029236775176431</v>
+        <v>1</v>
       </c>
       <c r="BS9">
-        <v>0.9064251525685132</v>
+        <v>1</v>
       </c>
       <c r="BT9">
-        <v>0.9079856497382467</v>
+        <v>1</v>
       </c>
       <c r="BU9">
-        <v>0.9199021145386702</v>
+        <v>1</v>
       </c>
       <c r="BV9">
-        <v>0.9401135734615098</v>
+        <v>1</v>
       </c>
       <c r="BW9">
-        <v>0.9661915227172601</v>
+        <v>1</v>
       </c>
       <c r="BX9">
-        <v>0.9711835444703134</v>
+        <v>1</v>
       </c>
       <c r="BY9">
-        <v>0.9813053600321811</v>
+        <v>1</v>
       </c>
       <c r="BZ9">
-        <v>0.9980544491015666</v>
+        <v>1</v>
       </c>
       <c r="CA9">
         <v>1</v>
@@ -8021,97 +8021,97 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.05644232829206049</v>
+        <v>0.05117150718014198</v>
       </c>
       <c r="E10">
-        <v>0.151119342891408</v>
+        <v>0.1750823723587365</v>
       </c>
       <c r="F10">
-        <v>0.1547892098311357</v>
+        <v>0.1750823723587365</v>
       </c>
       <c r="G10">
-        <v>0.1547892098311357</v>
+        <v>0.1750823723587365</v>
       </c>
       <c r="H10">
-        <v>0.1547892098311357</v>
+        <v>0.1750823723587365</v>
       </c>
       <c r="I10">
-        <v>0.1620940262262354</v>
+        <v>0.1750823723587365</v>
       </c>
       <c r="J10">
-        <v>0.1903597538701372</v>
+        <v>0.1750823723587365</v>
       </c>
       <c r="K10">
-        <v>0.1946638921694472</v>
+        <v>0.1750823723587365</v>
       </c>
       <c r="L10">
-        <v>0.2257036667543539</v>
+        <v>0.1779269380457712</v>
       </c>
       <c r="M10">
-        <v>0.2728425973519017</v>
+        <v>0.2113992500484137</v>
       </c>
       <c r="N10">
-        <v>0.272893001441503</v>
+        <v>0.2113992500484137</v>
       </c>
       <c r="O10">
-        <v>0.272893001441503</v>
+        <v>0.2113992500484137</v>
       </c>
       <c r="P10">
-        <v>0.272893001441503</v>
+        <v>0.2113992500484137</v>
       </c>
       <c r="Q10">
-        <v>0.272893001441503</v>
+        <v>0.2113992500484137</v>
       </c>
       <c r="R10">
-        <v>0.2876372654537566</v>
+        <v>0.2113992500484137</v>
       </c>
       <c r="S10">
-        <v>0.3164081858602671</v>
+        <v>0.2113992500484137</v>
       </c>
       <c r="T10">
-        <v>0.3845147392642719</v>
+        <v>0.2847612948825957</v>
       </c>
       <c r="U10">
-        <v>0.3989589252044545</v>
+        <v>0.2847612948825957</v>
       </c>
       <c r="V10">
-        <v>0.414285015316272</v>
+        <v>0.2847612948825957</v>
       </c>
       <c r="W10">
-        <v>0.5356398154679161</v>
+        <v>0.4594251590082381</v>
       </c>
       <c r="X10">
-        <v>0.6930566762765475</v>
+        <v>0.7026950820200125</v>
       </c>
       <c r="Y10">
-        <v>0.8331258317067759</v>
+        <v>0.9129619631909321</v>
       </c>
       <c r="Z10">
-        <v>0.8920420430666072</v>
+        <v>0.9688398949162284</v>
       </c>
       <c r="AA10">
-        <v>0.9035321465505388</v>
+        <v>0.9688398949162284</v>
       </c>
       <c r="AB10">
-        <v>0.907783909128028</v>
+        <v>0.9688398949162284</v>
       </c>
       <c r="AC10">
-        <v>0.907783909128028</v>
+        <v>0.9688398949162284</v>
       </c>
       <c r="AD10">
-        <v>0.9101508859652977</v>
+        <v>0.9688398949162284</v>
       </c>
       <c r="AE10">
-        <v>0.9167484904786294</v>
+        <v>0.9688398949162284</v>
       </c>
       <c r="AF10">
-        <v>0.9188674183962445</v>
+        <v>0.9688398949162284</v>
       </c>
       <c r="AG10">
-        <v>0.9323744571139031</v>
+        <v>0.9688398949162284</v>
       </c>
       <c r="AH10">
-        <v>0.9540764568990321</v>
+        <v>0.9688398949162284</v>
       </c>
       <c r="AI10">
         <v>1</v>
@@ -8632,97 +8632,97 @@
         <v>0</v>
       </c>
       <c r="CJ11">
-        <v>0.2617457971327486</v>
+        <v>0.4217467650485255</v>
       </c>
       <c r="CK11">
-        <v>0.2824729394783432</v>
+        <v>0.4217467650485255</v>
       </c>
       <c r="CL11">
-        <v>0.4720445309084161</v>
+        <v>0.7121460012457981</v>
       </c>
       <c r="CM11">
-        <v>0.5068612249106335</v>
+        <v>0.7209117486241643</v>
       </c>
       <c r="CN11">
-        <v>0.5348247352026579</v>
+        <v>0.7209117486241643</v>
       </c>
       <c r="CO11">
-        <v>0.5591896102152575</v>
+        <v>0.7209117486241643</v>
       </c>
       <c r="CP11">
-        <v>0.5735565180735449</v>
+        <v>0.7209117486241643</v>
       </c>
       <c r="CQ11">
-        <v>0.5834546140089832</v>
+        <v>0.7209117486241643</v>
       </c>
       <c r="CR11">
-        <v>0.5839934829844221</v>
+        <v>0.7209117486241643</v>
       </c>
       <c r="CS11">
-        <v>0.5897549797219304</v>
+        <v>0.7209117486241643</v>
       </c>
       <c r="CT11">
-        <v>0.6290036429587775</v>
+        <v>0.7377430950797341</v>
       </c>
       <c r="CU11">
-        <v>0.7307183831558134</v>
+        <v>0.8682544573508268</v>
       </c>
       <c r="CV11">
-        <v>0.7407765525236056</v>
+        <v>0.8682544573508268</v>
       </c>
       <c r="CW11">
-        <v>0.7894302433974725</v>
+        <v>0.9022017128333591</v>
       </c>
       <c r="CX11">
-        <v>0.8031572175157164</v>
+        <v>0.9022017128333591</v>
       </c>
       <c r="CY11">
-        <v>0.8592558505314458</v>
+        <v>0.9496977804330984</v>
       </c>
       <c r="CZ11">
-        <v>0.8725978125625801</v>
+        <v>0.9496977804330984</v>
       </c>
       <c r="DA11">
-        <v>0.9302383991352758</v>
+        <v>1</v>
       </c>
       <c r="DB11">
-        <v>0.9302770016617938</v>
+        <v>1</v>
       </c>
       <c r="DC11">
-        <v>0.9311153859667494</v>
+        <v>1</v>
       </c>
       <c r="DD11">
-        <v>0.9422181889611247</v>
+        <v>1</v>
       </c>
       <c r="DE11">
-        <v>0.9447992823697953</v>
+        <v>1</v>
       </c>
       <c r="DF11">
-        <v>0.9604696824596753</v>
+        <v>1</v>
       </c>
       <c r="DG11">
-        <v>0.971584933129544</v>
+        <v>1</v>
       </c>
       <c r="DH11">
-        <v>0.9719509218089677</v>
+        <v>1</v>
       </c>
       <c r="DI11">
-        <v>0.9738204498087532</v>
+        <v>1</v>
       </c>
       <c r="DJ11">
-        <v>0.987514790047755</v>
+        <v>1</v>
       </c>
       <c r="DK11">
-        <v>0.9919544920088165</v>
+        <v>1</v>
       </c>
       <c r="DL11">
-        <v>0.9927999520526923</v>
+        <v>1</v>
       </c>
       <c r="DM11">
-        <v>0.9966718037941394</v>
+        <v>1</v>
       </c>
       <c r="DN11">
-        <v>0.9994670906030334</v>
+        <v>1</v>
       </c>
       <c r="DO11">
         <v>1</v>
@@ -8787,34 +8787,34 @@
         <v>119</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>83</v>
       </c>
       <c r="D2">
-        <v>87</v>
+        <v>0.5</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.6792054419701443</v>
       </c>
       <c r="F2">
-        <v>0.596791837741518</v>
+        <v>86</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>800</v>
       </c>
       <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2">
         <v>12</v>
-      </c>
-      <c r="I2">
-        <v>800</v>
-      </c>
-      <c r="J2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" t="s">
-        <v>142</v>
       </c>
       <c r="L2" t="s">
         <v>143</v>
@@ -8828,34 +8828,34 @@
         <v>120</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>83</v>
       </c>
       <c r="D3">
-        <v>88</v>
+        <v>0.5</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.6256156386369657</v>
       </c>
       <c r="F3">
-        <v>0.5033074694108111</v>
+        <v>86</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>800</v>
       </c>
       <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K3">
         <v>12</v>
-      </c>
-      <c r="I3">
-        <v>800</v>
-      </c>
-      <c r="J3" t="s">
-        <v>141</v>
-      </c>
-      <c r="K3" t="s">
-        <v>142</v>
       </c>
       <c r="L3" t="s">
         <v>143</v>
@@ -8869,34 +8869,34 @@
         <v>121</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>84</v>
       </c>
       <c r="D4">
-        <v>97</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.5791477709263932</v>
       </c>
       <c r="F4">
-        <v>0.5935404464725584</v>
+        <v>88</v>
       </c>
       <c r="G4">
-        <v>13</v>
+        <v>800</v>
       </c>
       <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4">
         <v>12</v>
-      </c>
-      <c r="I4">
-        <v>800</v>
-      </c>
-      <c r="J4" t="s">
-        <v>141</v>
-      </c>
-      <c r="K4" t="s">
-        <v>142</v>
       </c>
       <c r="L4" t="s">
         <v>143</v>
@@ -8910,34 +8910,34 @@
         <v>122</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>84</v>
       </c>
       <c r="D5">
-        <v>91</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.6755416925685236</v>
       </c>
       <c r="F5">
-        <v>0.5112661015894928</v>
+        <v>88</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>800</v>
       </c>
       <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5">
         <v>12</v>
-      </c>
-      <c r="I5">
-        <v>800</v>
-      </c>
-      <c r="J5" t="s">
-        <v>141</v>
-      </c>
-      <c r="K5" t="s">
-        <v>142</v>
       </c>
       <c r="L5" t="s">
         <v>143</v>
@@ -8951,34 +8951,34 @@
         <v>123</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>83</v>
       </c>
       <c r="D6">
-        <v>96</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.506230210238605</v>
       </c>
       <c r="F6">
-        <v>0.6210275634083369</v>
+        <v>87</v>
       </c>
       <c r="G6">
-        <v>13</v>
+        <v>800</v>
       </c>
       <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K6">
         <v>12</v>
-      </c>
-      <c r="I6">
-        <v>800</v>
-      </c>
-      <c r="J6" t="s">
-        <v>141</v>
-      </c>
-      <c r="K6" t="s">
-        <v>142</v>
       </c>
       <c r="L6" t="s">
         <v>143</v>
@@ -8992,34 +8992,34 @@
         <v>124</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>83</v>
       </c>
       <c r="D7">
-        <v>89</v>
+        <v>0.5</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.6991421691795358</v>
       </c>
       <c r="F7">
-        <v>0.5089502041521814</v>
+        <v>87</v>
       </c>
       <c r="G7">
-        <v>6</v>
+        <v>800</v>
       </c>
       <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7">
         <v>12</v>
-      </c>
-      <c r="I7">
-        <v>800</v>
-      </c>
-      <c r="J7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" t="s">
-        <v>142</v>
       </c>
       <c r="L7" t="s">
         <v>143</v>
@@ -9033,34 +9033,34 @@
         <v>125</v>
       </c>
       <c r="B8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>83</v>
       </c>
       <c r="D8">
-        <v>91</v>
+        <v>0.5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.6268833330636873</v>
       </c>
       <c r="F8">
-        <v>0.5151338581037042</v>
+        <v>87</v>
       </c>
       <c r="G8">
-        <v>8</v>
+        <v>800</v>
       </c>
       <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8">
         <v>12</v>
-      </c>
-      <c r="I8">
-        <v>800</v>
-      </c>
-      <c r="J8" t="s">
-        <v>141</v>
-      </c>
-      <c r="K8" t="s">
-        <v>142</v>
       </c>
       <c r="L8" t="s">
         <v>143</v>
@@ -9074,34 +9074,34 @@
         <v>126</v>
       </c>
       <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>46</v>
+      </c>
+      <c r="D9">
         <v>0.5</v>
       </c>
-      <c r="C9">
-        <v>45</v>
-      </c>
-      <c r="D9">
-        <v>56</v>
-      </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.5430169115523709</v>
       </c>
       <c r="F9">
-        <v>0.5102714452676769</v>
+        <v>49</v>
       </c>
       <c r="G9">
-        <v>11</v>
+        <v>800</v>
       </c>
       <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9">
         <v>12</v>
-      </c>
-      <c r="I9">
-        <v>800</v>
-      </c>
-      <c r="J9" t="s">
-        <v>141</v>
-      </c>
-      <c r="K9" t="s">
-        <v>142</v>
       </c>
       <c r="L9" t="s">
         <v>143</v>
@@ -9115,34 +9115,34 @@
         <v>127</v>
       </c>
       <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>0.5</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
+      <c r="E10">
+        <v>0.7026950820200125</v>
+      </c>
+      <c r="F10">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <v>800</v>
+      </c>
+      <c r="H10">
         <v>22</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0.5356398154679161</v>
-      </c>
-      <c r="G10">
-        <v>21</v>
-      </c>
-      <c r="H10">
+      <c r="I10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K10">
         <v>12</v>
-      </c>
-      <c r="I10">
-        <v>800</v>
-      </c>
-      <c r="J10" t="s">
-        <v>141</v>
-      </c>
-      <c r="K10" t="s">
-        <v>142</v>
       </c>
       <c r="L10" t="s">
         <v>143</v>
@@ -9156,34 +9156,34 @@
         <v>128</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>85</v>
       </c>
       <c r="D11">
-        <v>90</v>
+        <v>0.5</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.7121460012457981</v>
       </c>
       <c r="F11">
-        <v>0.5068612249106335</v>
+        <v>89</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>800</v>
       </c>
       <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>141</v>
+      </c>
+      <c r="J11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11">
         <v>12</v>
-      </c>
-      <c r="I11">
-        <v>800</v>
-      </c>
-      <c r="J11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K11" t="s">
-        <v>142</v>
       </c>
       <c r="L11" t="s">
         <v>143</v>
@@ -9251,34 +9251,34 @@
         <v>119</v>
       </c>
       <c r="B2">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>83</v>
       </c>
       <c r="D2">
-        <v>96</v>
+        <v>0.7</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.7921127441701877</v>
       </c>
       <c r="F2">
-        <v>0.8143637124523496</v>
+        <v>87</v>
       </c>
       <c r="G2">
-        <v>13</v>
+        <v>800</v>
       </c>
       <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2">
         <v>12</v>
-      </c>
-      <c r="I2">
-        <v>800</v>
-      </c>
-      <c r="J2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" t="s">
-        <v>142</v>
       </c>
       <c r="L2" t="s">
         <v>143</v>
@@ -9292,34 +9292,34 @@
         <v>120</v>
       </c>
       <c r="B3">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>83</v>
       </c>
       <c r="D3">
-        <v>96</v>
+        <v>0.7</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.707620123004011</v>
       </c>
       <c r="F3">
-        <v>0.7576194513916251</v>
+        <v>87</v>
       </c>
       <c r="G3">
-        <v>13</v>
+        <v>800</v>
       </c>
       <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K3">
         <v>12</v>
-      </c>
-      <c r="I3">
-        <v>800</v>
-      </c>
-      <c r="J3" t="s">
-        <v>141</v>
-      </c>
-      <c r="K3" t="s">
-        <v>142</v>
       </c>
       <c r="L3" t="s">
         <v>143</v>
@@ -9333,34 +9333,34 @@
         <v>121</v>
       </c>
       <c r="B4">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>84</v>
       </c>
       <c r="D4">
-        <v>98</v>
+        <v>0.7</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.7398275006750992</v>
       </c>
       <c r="F4">
-        <v>0.7109084531338365</v>
+        <v>97</v>
       </c>
       <c r="G4">
-        <v>14</v>
+        <v>800</v>
       </c>
       <c r="H4">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4">
         <v>12</v>
-      </c>
-      <c r="I4">
-        <v>800</v>
-      </c>
-      <c r="J4" t="s">
-        <v>141</v>
-      </c>
-      <c r="K4" t="s">
-        <v>142</v>
       </c>
       <c r="L4" t="s">
         <v>143</v>
@@ -9374,34 +9374,34 @@
         <v>122</v>
       </c>
       <c r="B5">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>84</v>
       </c>
       <c r="D5">
-        <v>98</v>
+        <v>0.7</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.7850887754613128</v>
       </c>
       <c r="F5">
-        <v>0.7033332573165157</v>
+        <v>97</v>
       </c>
       <c r="G5">
-        <v>14</v>
+        <v>800</v>
       </c>
       <c r="H5">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5">
         <v>12</v>
-      </c>
-      <c r="I5">
-        <v>800</v>
-      </c>
-      <c r="J5" t="s">
-        <v>141</v>
-      </c>
-      <c r="K5" t="s">
-        <v>142</v>
       </c>
       <c r="L5" t="s">
         <v>143</v>
@@ -9415,34 +9415,34 @@
         <v>123</v>
       </c>
       <c r="B6">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>83</v>
       </c>
       <c r="D6">
+        <v>0.7</v>
+      </c>
+      <c r="E6">
+        <v>0.8412839469765355</v>
+      </c>
+      <c r="F6">
         <v>98</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0.7705380677611648</v>
-      </c>
       <c r="G6">
+        <v>800</v>
+      </c>
+      <c r="H6">
         <v>15</v>
       </c>
-      <c r="H6">
+      <c r="I6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K6">
         <v>12</v>
-      </c>
-      <c r="I6">
-        <v>800</v>
-      </c>
-      <c r="J6" t="s">
-        <v>141</v>
-      </c>
-      <c r="K6" t="s">
-        <v>142</v>
       </c>
       <c r="L6" t="s">
         <v>143</v>
@@ -9456,34 +9456,34 @@
         <v>124</v>
       </c>
       <c r="B7">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>83</v>
       </c>
       <c r="D7">
-        <v>96</v>
+        <v>0.7</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.7559258084701969</v>
       </c>
       <c r="F7">
-        <v>0.7304060613318696</v>
+        <v>90</v>
       </c>
       <c r="G7">
-        <v>13</v>
+        <v>800</v>
       </c>
       <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7">
         <v>12</v>
-      </c>
-      <c r="I7">
-        <v>800</v>
-      </c>
-      <c r="J7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" t="s">
-        <v>142</v>
       </c>
       <c r="L7" t="s">
         <v>143</v>
@@ -9497,34 +9497,34 @@
         <v>125</v>
       </c>
       <c r="B8">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>83</v>
       </c>
       <c r="D8">
-        <v>97</v>
+        <v>0.7</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.7908929189186144</v>
       </c>
       <c r="F8">
-        <v>0.7055349613624133</v>
+        <v>96</v>
       </c>
       <c r="G8">
-        <v>14</v>
+        <v>800</v>
       </c>
       <c r="H8">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8">
         <v>12</v>
-      </c>
-      <c r="I8">
-        <v>800</v>
-      </c>
-      <c r="J8" t="s">
-        <v>141</v>
-      </c>
-      <c r="K8" t="s">
-        <v>142</v>
       </c>
       <c r="L8" t="s">
         <v>143</v>
@@ -9538,34 +9538,34 @@
         <v>126</v>
       </c>
       <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>46</v>
+      </c>
+      <c r="D9">
         <v>0.7</v>
       </c>
-      <c r="C9">
-        <v>45</v>
-      </c>
-      <c r="D9">
+      <c r="E9">
+        <v>0.8851766969236824</v>
+      </c>
+      <c r="F9">
         <v>59</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0.7053049228115669</v>
-      </c>
       <c r="G9">
-        <v>14</v>
+        <v>800</v>
       </c>
       <c r="H9">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9">
         <v>12</v>
-      </c>
-      <c r="I9">
-        <v>800</v>
-      </c>
-      <c r="J9" t="s">
-        <v>141</v>
-      </c>
-      <c r="K9" t="s">
-        <v>142</v>
       </c>
       <c r="L9" t="s">
         <v>143</v>
@@ -9579,34 +9579,34 @@
         <v>127</v>
       </c>
       <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>0.7</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>24</v>
-      </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.7026950820200125</v>
       </c>
       <c r="F10">
-        <v>0.8331258317067759</v>
+        <v>23</v>
       </c>
       <c r="G10">
-        <v>23</v>
+        <v>800</v>
       </c>
       <c r="H10">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K10">
         <v>12</v>
-      </c>
-      <c r="I10">
-        <v>800</v>
-      </c>
-      <c r="J10" t="s">
-        <v>141</v>
-      </c>
-      <c r="K10" t="s">
-        <v>142</v>
       </c>
       <c r="L10" t="s">
         <v>143</v>
@@ -9620,34 +9620,34 @@
         <v>128</v>
       </c>
       <c r="B11">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>85</v>
       </c>
       <c r="D11">
-        <v>98</v>
+        <v>0.7</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.7121460012457981</v>
       </c>
       <c r="F11">
-        <v>0.7307183831558134</v>
+        <v>89</v>
       </c>
       <c r="G11">
-        <v>13</v>
+        <v>800</v>
       </c>
       <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>141</v>
+      </c>
+      <c r="J11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11">
         <v>12</v>
-      </c>
-      <c r="I11">
-        <v>800</v>
-      </c>
-      <c r="J11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K11" t="s">
-        <v>142</v>
       </c>
       <c r="L11" t="s">
         <v>143</v>
@@ -9715,34 +9715,34 @@
         <v>119</v>
       </c>
       <c r="B2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>83</v>
       </c>
       <c r="D2">
-        <v>96</v>
+        <v>0.8</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.8037670542964901</v>
       </c>
       <c r="F2">
-        <v>0.8143637124523496</v>
+        <v>89</v>
       </c>
       <c r="G2">
-        <v>13</v>
+        <v>800</v>
       </c>
       <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2">
         <v>12</v>
-      </c>
-      <c r="I2">
-        <v>800</v>
-      </c>
-      <c r="J2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" t="s">
-        <v>142</v>
       </c>
       <c r="L2" t="s">
         <v>143</v>
@@ -9756,34 +9756,34 @@
         <v>120</v>
       </c>
       <c r="B3">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>83</v>
       </c>
       <c r="D3">
-        <v>98</v>
+        <v>0.8</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.9072835186536428</v>
       </c>
       <c r="F3">
-        <v>0.8302273868702849</v>
+        <v>96</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>800</v>
       </c>
       <c r="H3">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K3">
         <v>12</v>
-      </c>
-      <c r="I3">
-        <v>800</v>
-      </c>
-      <c r="J3" t="s">
-        <v>141</v>
-      </c>
-      <c r="K3" t="s">
-        <v>142</v>
       </c>
       <c r="L3" t="s">
         <v>143</v>
@@ -9797,34 +9797,34 @@
         <v>121</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>84</v>
       </c>
       <c r="D4">
-        <v>101</v>
+        <v>0.8</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.9026387446873847</v>
       </c>
       <c r="F4">
-        <v>0.8350982804078538</v>
+        <v>98</v>
       </c>
       <c r="G4">
-        <v>17</v>
+        <v>800</v>
       </c>
       <c r="H4">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4">
         <v>12</v>
-      </c>
-      <c r="I4">
-        <v>800</v>
-      </c>
-      <c r="J4" t="s">
-        <v>141</v>
-      </c>
-      <c r="K4" t="s">
-        <v>142</v>
       </c>
       <c r="L4" t="s">
         <v>143</v>
@@ -9838,34 +9838,34 @@
         <v>122</v>
       </c>
       <c r="B5">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>84</v>
       </c>
       <c r="D5">
-        <v>101</v>
+        <v>0.8</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.8663140912976856</v>
       </c>
       <c r="F5">
-        <v>0.8485572460934055</v>
+        <v>98</v>
       </c>
       <c r="G5">
-        <v>17</v>
+        <v>800</v>
       </c>
       <c r="H5">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5">
         <v>12</v>
-      </c>
-      <c r="I5">
-        <v>800</v>
-      </c>
-      <c r="J5" t="s">
-        <v>141</v>
-      </c>
-      <c r="K5" t="s">
-        <v>142</v>
       </c>
       <c r="L5" t="s">
         <v>143</v>
@@ -9879,34 +9879,34 @@
         <v>123</v>
       </c>
       <c r="B6">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>83</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>0.8</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.8412839469765355</v>
       </c>
       <c r="F6">
-        <v>0.8912594925293911</v>
+        <v>98</v>
       </c>
       <c r="G6">
-        <v>17</v>
+        <v>800</v>
       </c>
       <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K6">
         <v>12</v>
-      </c>
-      <c r="I6">
-        <v>800</v>
-      </c>
-      <c r="J6" t="s">
-        <v>141</v>
-      </c>
-      <c r="K6" t="s">
-        <v>142</v>
       </c>
       <c r="L6" t="s">
         <v>143</v>
@@ -9920,34 +9920,34 @@
         <v>124</v>
       </c>
       <c r="B7">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>83</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>0.8</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.8971976513541992</v>
       </c>
       <c r="F7">
-        <v>0.8668755778102364</v>
+        <v>96</v>
       </c>
       <c r="G7">
-        <v>17</v>
+        <v>800</v>
       </c>
       <c r="H7">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7">
         <v>12</v>
-      </c>
-      <c r="I7">
-        <v>800</v>
-      </c>
-      <c r="J7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" t="s">
-        <v>142</v>
       </c>
       <c r="L7" t="s">
         <v>143</v>
@@ -9961,34 +9961,34 @@
         <v>125</v>
       </c>
       <c r="B8">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>83</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>0.8</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.8215860976803671</v>
       </c>
       <c r="F8">
-        <v>0.8602783545050369</v>
+        <v>97</v>
       </c>
       <c r="G8">
-        <v>17</v>
+        <v>800</v>
       </c>
       <c r="H8">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8">
         <v>12</v>
-      </c>
-      <c r="I8">
-        <v>800</v>
-      </c>
-      <c r="J8" t="s">
-        <v>141</v>
-      </c>
-      <c r="K8" t="s">
-        <v>142</v>
       </c>
       <c r="L8" t="s">
         <v>143</v>
@@ -10002,34 +10002,34 @@
         <v>126</v>
       </c>
       <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>46</v>
+      </c>
+      <c r="D9">
         <v>0.8</v>
       </c>
-      <c r="C9">
-        <v>45</v>
-      </c>
-      <c r="D9">
-        <v>63</v>
-      </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.8851766969236824</v>
       </c>
       <c r="F9">
-        <v>0.838978356780303</v>
+        <v>59</v>
       </c>
       <c r="G9">
-        <v>18</v>
+        <v>800</v>
       </c>
       <c r="H9">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9">
         <v>12</v>
-      </c>
-      <c r="I9">
-        <v>800</v>
-      </c>
-      <c r="J9" t="s">
-        <v>141</v>
-      </c>
-      <c r="K9" t="s">
-        <v>142</v>
       </c>
       <c r="L9" t="s">
         <v>143</v>
@@ -10043,34 +10043,34 @@
         <v>127</v>
       </c>
       <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>0.8</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
+      <c r="E10">
+        <v>0.9129619631909321</v>
+      </c>
+      <c r="F10">
         <v>24</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0.8331258317067759</v>
-      </c>
       <c r="G10">
+        <v>800</v>
+      </c>
+      <c r="H10">
         <v>23</v>
       </c>
-      <c r="H10">
+      <c r="I10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K10">
         <v>12</v>
-      </c>
-      <c r="I10">
-        <v>800</v>
-      </c>
-      <c r="J10" t="s">
-        <v>141</v>
-      </c>
-      <c r="K10" t="s">
-        <v>142</v>
       </c>
       <c r="L10" t="s">
         <v>143</v>
@@ -10084,34 +10084,34 @@
         <v>128</v>
       </c>
       <c r="B11">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>85</v>
       </c>
       <c r="D11">
-        <v>101</v>
+        <v>0.8</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.8682544573508268</v>
       </c>
       <c r="F11">
-        <v>0.8031572175157164</v>
+        <v>98</v>
       </c>
       <c r="G11">
-        <v>16</v>
+        <v>800</v>
       </c>
       <c r="H11">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>141</v>
+      </c>
+      <c r="J11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11">
         <v>12</v>
-      </c>
-      <c r="I11">
-        <v>800</v>
-      </c>
-      <c r="J11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K11" t="s">
-        <v>142</v>
       </c>
       <c r="L11" t="s">
         <v>143</v>
@@ -10179,34 +10179,34 @@
         <v>119</v>
       </c>
       <c r="B2">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>83</v>
       </c>
       <c r="D2">
-        <v>101</v>
+        <v>0.9</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.9675276807434803</v>
       </c>
       <c r="F2">
-        <v>0.9106504043751427</v>
+        <v>96</v>
       </c>
       <c r="G2">
-        <v>18</v>
+        <v>800</v>
       </c>
       <c r="H2">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2">
         <v>12</v>
-      </c>
-      <c r="I2">
-        <v>800</v>
-      </c>
-      <c r="J2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" t="s">
-        <v>142</v>
       </c>
       <c r="L2" t="s">
         <v>143</v>
@@ -10220,34 +10220,34 @@
         <v>120</v>
       </c>
       <c r="B3">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>83</v>
       </c>
       <c r="D3">
-        <v>101</v>
+        <v>0.9</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.9072835186536428</v>
       </c>
       <c r="F3">
-        <v>0.90403291226872</v>
+        <v>96</v>
       </c>
       <c r="G3">
-        <v>18</v>
+        <v>800</v>
       </c>
       <c r="H3">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K3">
         <v>12</v>
-      </c>
-      <c r="I3">
-        <v>800</v>
-      </c>
-      <c r="J3" t="s">
-        <v>141</v>
-      </c>
-      <c r="K3" t="s">
-        <v>142</v>
       </c>
       <c r="L3" t="s">
         <v>143</v>
@@ -10261,34 +10261,34 @@
         <v>121</v>
       </c>
       <c r="B4">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>84</v>
       </c>
       <c r="D4">
-        <v>106</v>
+        <v>0.9</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.9026387446873847</v>
       </c>
       <c r="F4">
-        <v>0.9075427803747935</v>
+        <v>98</v>
       </c>
       <c r="G4">
-        <v>22</v>
+        <v>800</v>
       </c>
       <c r="H4">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4">
         <v>12</v>
-      </c>
-      <c r="I4">
-        <v>800</v>
-      </c>
-      <c r="J4" t="s">
-        <v>141</v>
-      </c>
-      <c r="K4" t="s">
-        <v>142</v>
       </c>
       <c r="L4" t="s">
         <v>143</v>
@@ -10302,34 +10302,34 @@
         <v>122</v>
       </c>
       <c r="B5">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>84</v>
       </c>
       <c r="D5">
-        <v>106</v>
+        <v>0.9</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0.910867452492105</v>
+        <v>101</v>
       </c>
       <c r="G5">
-        <v>22</v>
+        <v>800</v>
       </c>
       <c r="H5">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5">
         <v>12</v>
-      </c>
-      <c r="I5">
-        <v>800</v>
-      </c>
-      <c r="J5" t="s">
-        <v>141</v>
-      </c>
-      <c r="K5" t="s">
-        <v>142</v>
       </c>
       <c r="L5" t="s">
         <v>143</v>
@@ -10343,34 +10343,34 @@
         <v>123</v>
       </c>
       <c r="B6">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>83</v>
       </c>
       <c r="D6">
-        <v>101</v>
+        <v>0.9</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0.9199374231532217</v>
+        <v>100</v>
       </c>
       <c r="G6">
-        <v>18</v>
+        <v>800</v>
       </c>
       <c r="H6">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K6">
         <v>12</v>
-      </c>
-      <c r="I6">
-        <v>800</v>
-      </c>
-      <c r="J6" t="s">
-        <v>141</v>
-      </c>
-      <c r="K6" t="s">
-        <v>142</v>
       </c>
       <c r="L6" t="s">
         <v>143</v>
@@ -10384,34 +10384,34 @@
         <v>124</v>
       </c>
       <c r="B7">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>83</v>
       </c>
       <c r="D7">
-        <v>102</v>
+        <v>0.9</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.9294255975524877</v>
       </c>
       <c r="F7">
-        <v>0.9078030919533135</v>
+        <v>98</v>
       </c>
       <c r="G7">
-        <v>19</v>
+        <v>800</v>
       </c>
       <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7">
         <v>12</v>
-      </c>
-      <c r="I7">
-        <v>800</v>
-      </c>
-      <c r="J7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" t="s">
-        <v>142</v>
       </c>
       <c r="L7" t="s">
         <v>143</v>
@@ -10425,34 +10425,34 @@
         <v>125</v>
       </c>
       <c r="B8">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>83</v>
       </c>
       <c r="D8">
-        <v>102</v>
+        <v>0.9</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.9598319356202181</v>
       </c>
       <c r="F8">
-        <v>0.9121411786830566</v>
+        <v>100</v>
       </c>
       <c r="G8">
-        <v>19</v>
+        <v>800</v>
       </c>
       <c r="H8">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8">
         <v>12</v>
-      </c>
-      <c r="I8">
-        <v>800</v>
-      </c>
-      <c r="J8" t="s">
-        <v>141</v>
-      </c>
-      <c r="K8" t="s">
-        <v>142</v>
       </c>
       <c r="L8" t="s">
         <v>143</v>
@@ -10466,34 +10466,34 @@
         <v>126</v>
       </c>
       <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>46</v>
+      </c>
+      <c r="D9">
         <v>0.9</v>
       </c>
-      <c r="C9">
-        <v>45</v>
-      </c>
-      <c r="D9">
-        <v>69</v>
-      </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.902166397301188</v>
       </c>
       <c r="F9">
-        <v>0.9029236775176431</v>
+        <v>61</v>
       </c>
       <c r="G9">
-        <v>24</v>
+        <v>800</v>
       </c>
       <c r="H9">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9">
         <v>12</v>
-      </c>
-      <c r="I9">
-        <v>800</v>
-      </c>
-      <c r="J9" t="s">
-        <v>141</v>
-      </c>
-      <c r="K9" t="s">
-        <v>142</v>
       </c>
       <c r="L9" t="s">
         <v>143</v>
@@ -10507,34 +10507,34 @@
         <v>127</v>
       </c>
       <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>0.9</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>26</v>
-      </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.9129619631909321</v>
       </c>
       <c r="F10">
-        <v>0.9035321465505388</v>
+        <v>24</v>
       </c>
       <c r="G10">
-        <v>25</v>
+        <v>800</v>
       </c>
       <c r="H10">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K10">
         <v>12</v>
-      </c>
-      <c r="I10">
-        <v>800</v>
-      </c>
-      <c r="J10" t="s">
-        <v>141</v>
-      </c>
-      <c r="K10" t="s">
-        <v>142</v>
       </c>
       <c r="L10" t="s">
         <v>143</v>
@@ -10548,34 +10548,34 @@
         <v>128</v>
       </c>
       <c r="B11">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>85</v>
       </c>
       <c r="D11">
-        <v>104</v>
+        <v>0.9</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.9022017128333591</v>
       </c>
       <c r="F11">
-        <v>0.9302383991352758</v>
+        <v>100</v>
       </c>
       <c r="G11">
-        <v>19</v>
+        <v>800</v>
       </c>
       <c r="H11">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>141</v>
+      </c>
+      <c r="J11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11">
         <v>12</v>
-      </c>
-      <c r="I11">
-        <v>800</v>
-      </c>
-      <c r="J11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K11" t="s">
-        <v>142</v>
       </c>
       <c r="L11" t="s">
         <v>143</v>

</xml_diff>